<commit_message>
Atualiza planilha, script e adiciona logo Mercado Livre
</commit_message>
<xml_diff>
--- a/lat-long.xlsx
+++ b/lat-long.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamarra\Documents\PROJETOS\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43D8266-5C80-4E7A-BFEB-019C2E3E4266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F69581-8317-4BF7-A413-385861EFE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B20DCDFB-8054-47D0-956B-6BBF474CFB0A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="564">
   <si>
     <t>lat</t>
   </si>
@@ -1274,6 +1274,459 @@
   </si>
   <si>
     <t>4109, Avenida Presidente Kennedy, Parolin, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Camões, Hugo Lange, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80040-320, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Camões</t>
+  </si>
+  <si>
+    <t>Hugo Lange</t>
+  </si>
+  <si>
+    <t>80040-320</t>
+  </si>
+  <si>
+    <t>Rua 24 de Maio, Rebouças, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80230-090, Brasil</t>
+  </si>
+  <si>
+    <t>80230-090</t>
+  </si>
+  <si>
+    <t>847, Rua Rockefeller, Rebouças, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80230-130, Brasil</t>
+  </si>
+  <si>
+    <t>41, Rua Lamenha Lins, Centro, Curitiba, Curitiba, Paraná, 80250-020, Brasil</t>
+  </si>
+  <si>
+    <t>80250-020</t>
+  </si>
+  <si>
+    <t>Rua José Naves da Cunha, Seminário, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80310-100, Brasil</t>
+  </si>
+  <si>
+    <t>Rua José Naves da Cunha</t>
+  </si>
+  <si>
+    <t>80310-100</t>
+  </si>
+  <si>
+    <t>285, Avenida Vicente Machado, Centro, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80410-201, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Senador Xavier da Silva, Centro Cívico, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81450-360, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Senador Xavier da Silva</t>
+  </si>
+  <si>
+    <t>81450-360</t>
+  </si>
+  <si>
+    <t>2532, Avenida Presidente Kennedy, Água Verde, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80610-020, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Francisco Rocha, Bigorrilho, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80730-380, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Francisco Rocha</t>
+  </si>
+  <si>
+    <t>80730-380</t>
+  </si>
+  <si>
+    <t>Rua Clara Polsin, Novo Mundo, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81020-320, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Clara Polsin</t>
+  </si>
+  <si>
+    <t>81020-320</t>
+  </si>
+  <si>
+    <t>866, Rua Maestro Francisco Antonello, Fanny, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Coronel Herculano de Araújo, Novo Mundo, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81050-080, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Coronel Herculano de Araújo</t>
+  </si>
+  <si>
+    <t>Rua Itatiaia, Portão, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 80610-010, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Itatiaia</t>
+  </si>
+  <si>
+    <t>Rua Laudelino Ferreira Lopes, Capão Raso, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81130-290, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Laudelino Ferreira Lopes</t>
+  </si>
+  <si>
+    <t>Capão Raso</t>
+  </si>
+  <si>
+    <t>81130-290</t>
+  </si>
+  <si>
+    <t>Rua Nelson Ferreira da Luz, Campo Comprido, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81230-162, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Nelson Ferreira da Luz</t>
+  </si>
+  <si>
+    <t>Campo Comprido</t>
+  </si>
+  <si>
+    <t>81230-162</t>
+  </si>
+  <si>
+    <t>02461, R. Raul Pompeia, Cidade Industrial De Curitiba, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>R. Raul Pompeia</t>
+  </si>
+  <si>
+    <t>87, Avenida Padre Estanislau De Campos, Cidade Lider, São Paulo, São Paulo, São Paulo, 03590-060, Brasil</t>
+  </si>
+  <si>
+    <t>Avenida Padre Estanislau De Campos</t>
+  </si>
+  <si>
+    <t>Cidade Lider</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>03590-060</t>
+  </si>
+  <si>
+    <t>Rua Anselmo Fregonezi, Poços de Caldas, Poços de Caldas, Minas Gerais, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Anselmo Fregonezi</t>
+  </si>
+  <si>
+    <t>Poços de Caldas</t>
+  </si>
+  <si>
+    <t>Minas Gerais</t>
+  </si>
+  <si>
+    <t>Rua Maria Quitéria, Fazendinha, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81330-430, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Maria Quitéria</t>
+  </si>
+  <si>
+    <t>Fazendinha</t>
+  </si>
+  <si>
+    <t>81330-430</t>
+  </si>
+  <si>
+    <t>2781, Rua General Potiguara, Fazendinha, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81320-000, Brasil</t>
+  </si>
+  <si>
+    <t>Rua General Potiguara</t>
+  </si>
+  <si>
+    <t>81320-000</t>
+  </si>
+  <si>
+    <t>90, Rua Antonio Pastre, Cidade Industrial De Curitiba, Curitiba, Curitiba, Paraná, 81240-000, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Antonio Pastre</t>
+  </si>
+  <si>
+    <t>1047, Rua Odir Gomes da Rocha, Tatuquara, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81470-470, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Odir Gomes da Rocha</t>
+  </si>
+  <si>
+    <t>Rua Alda Bassetti Bertholdi, Moradias Rio Bonito, Campo de Santana, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 87483-001, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Alda Bassetti Bertholdi</t>
+  </si>
+  <si>
+    <t>Campo de Santana</t>
+  </si>
+  <si>
+    <t>87483-001</t>
+  </si>
+  <si>
+    <t>50, Rua Leonardo da Vinci, Guabirotuba, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Leonardo da Vinci</t>
+  </si>
+  <si>
+    <t>173, Rua Jose Moreira, Uberaba, Uberaba, Minas Gerais, 38082-261, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Jose Moreira</t>
+  </si>
+  <si>
+    <t>38082-261</t>
+  </si>
+  <si>
+    <t>5595, Avenida Marechal Floriano Peixoto, Hauer, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81630-000, Brasil</t>
+  </si>
+  <si>
+    <t>Hauer</t>
+  </si>
+  <si>
+    <t>81630-000</t>
+  </si>
+  <si>
+    <t>707, Rua Napoleão Laureano, Boqueirão, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81650-210, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Napoleão Laureano</t>
+  </si>
+  <si>
+    <t>81650-210</t>
+  </si>
+  <si>
+    <t>Rua Hipólito da Costa, Boqueirão, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81670-110, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Hipólito da Costa</t>
+  </si>
+  <si>
+    <t>81670-110</t>
+  </si>
+  <si>
+    <t>119, Rua Antonio Rebelatto, Xaxim, Xaxim, Santa Catarina, 89825-000, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Antonio Rebelatto</t>
+  </si>
+  <si>
+    <t>Santa Catarina</t>
+  </si>
+  <si>
+    <t>89825-000</t>
+  </si>
+  <si>
+    <t>975, Rua 1º de Maio, Jardim Urano, Xaxim, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81810-000, Brasil</t>
+  </si>
+  <si>
+    <t>Rua 1º de Maio</t>
+  </si>
+  <si>
+    <t>81810-000</t>
+  </si>
+  <si>
+    <t>79, Rua Monte Nebo, Alto Boqueirão, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Monte Nebo</t>
+  </si>
+  <si>
+    <t>Rua David Tows, Vila Jardim Coqueiros, Sítio Cercado, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81920-640, Brasil</t>
+  </si>
+  <si>
+    <t>81920-640</t>
+  </si>
+  <si>
+    <t>2433, Rua David Tows, Vila Jardim Coqueiros, Sítio Cercado, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81920-640, Brasil</t>
+  </si>
+  <si>
+    <t>Rua São José dos Pinhais, Sítio Cercado, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81920-500, Brasil</t>
+  </si>
+  <si>
+    <t>Rua São José dos Pinhais</t>
+  </si>
+  <si>
+    <t>81920-500</t>
+  </si>
+  <si>
+    <t>Rua Mandirituba, Sítio Cercado, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81925-540, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Guaçuí, Sítio Cercado, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81935-060, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Guaçuí</t>
+  </si>
+  <si>
+    <t>81935-060</t>
+  </si>
+  <si>
+    <t>Avenida Cândido Hartmann, Santa Felicidade, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81200-170, Brasil</t>
+  </si>
+  <si>
+    <t>Avenida Cândido Hartmann</t>
+  </si>
+  <si>
+    <t>81200-170</t>
+  </si>
+  <si>
+    <t>Rua Santa Bertila Boscardin, São João, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Raposo Tavares, Pilarzinho, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82100-510, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Raposo Tavares</t>
+  </si>
+  <si>
+    <t>82100-510</t>
+  </si>
+  <si>
+    <t>Rua Mateus Leme, Abranches, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82210-050, Brasil</t>
+  </si>
+  <si>
+    <t>Abranches</t>
+  </si>
+  <si>
+    <t>Rua Antônio Corrêa Bittencourt, Ahú, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82200-220, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Antônio Corrêa Bittencourt</t>
+  </si>
+  <si>
+    <t>Ahú</t>
+  </si>
+  <si>
+    <t>82200-220</t>
+  </si>
+  <si>
+    <t>2, Rua Professor Leonardo Cobbe, Barreirinha, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Professor Leonardo Cobbe</t>
+  </si>
+  <si>
+    <t>Beauty Color, 3225, Avenida Vereador Toaldo Túlio, São Braz, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82300-332, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Pedro Costa, Ângelo Frechiani, Colatina, Espírito Santo, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Pedro Costa</t>
+  </si>
+  <si>
+    <t>Ângelo Frechiani</t>
+  </si>
+  <si>
+    <t>Colatina</t>
+  </si>
+  <si>
+    <t>Espírito Santo</t>
+  </si>
+  <si>
+    <t>Rua João Reffo, Santa Felicidade, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82410-220, Brasil</t>
+  </si>
+  <si>
+    <t>82410-220</t>
+  </si>
+  <si>
+    <t>Rua Estados Unidos, Bacacheri, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82515-030, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Estados Unidos</t>
+  </si>
+  <si>
+    <t>82515-030</t>
+  </si>
+  <si>
+    <t>Rua Carlota Straube de Araújo, Boa Vista, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82650-090, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Carlota Straube de Araújo</t>
+  </si>
+  <si>
+    <t>90, Estrada De Santa Candida, Tinguí, Curitiba, Curitiba, Paraná, 83503-290, Brasil</t>
+  </si>
+  <si>
+    <t>Estrada De Santa Candida</t>
+  </si>
+  <si>
+    <t>83503-290</t>
+  </si>
+  <si>
+    <t>Santa Candida, Culiacán, Sinaloa, México</t>
+  </si>
+  <si>
+    <t>Santa Candida</t>
+  </si>
+  <si>
+    <t>Culiacán</t>
+  </si>
+  <si>
+    <t>Sinaloa</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>mx</t>
+  </si>
+  <si>
+    <t>Rua Coronel Domingos Soares, Bairro Alto, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82820-090, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Coronel Domingos Soares</t>
+  </si>
+  <si>
+    <t>Rua Percy Feliciano de Castilho, Bairro Alto, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82820-390, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Percy Feliciano de Castilho</t>
+  </si>
+  <si>
+    <t>82820-390</t>
+  </si>
+  <si>
+    <t>Rua Leonardo Novicki, Vila São Domingos Agrícola, Cajuru, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82930-548, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Leonardo Novicki</t>
+  </si>
+  <si>
+    <t>82930-548</t>
+  </si>
+  <si>
+    <t>1616, Rua Luiz França, Cajuru, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82950-070, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Luiz França</t>
+  </si>
+  <si>
+    <t>82950-070</t>
+  </si>
+  <si>
+    <t>Rua Engenheiro Benedito Mário da Silva, Cajuru, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 82970-232, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Engenheiro Benedito Mário da Silva</t>
+  </si>
+  <si>
+    <t>82970-232</t>
+  </si>
+  <si>
+    <t>4211, Rua Eduardo Sprada, Campo Comprido, Curitiba, Região Geográfica Imediata de Curitiba, Região Metropolitana de Curitiba, Região Geográfica Intermediária de Curitiba, Paraná, Região Sul, 81270-010, Brasil</t>
+  </si>
+  <si>
+    <t>Rua Eduardo Sprada</t>
+  </si>
+  <si>
+    <t>81270-010</t>
+  </si>
+  <si>
+    <t>01569, R. João Dembinski, Curitiba, Curitiba, Paraná, Brasil</t>
+  </si>
+  <si>
+    <t>R. João Dembinski</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1368,6 +1821,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1685,11 +2141,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955423F3-DE01-43AA-8F25-6FB4450205BF}">
-  <dimension ref="A1:U149"/>
+  <dimension ref="A1:U211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J149" sqref="J149"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V159" sqref="V159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9196,6 +9652,3068 @@
         <v>28</v>
       </c>
       <c r="T149" s="5"/>
+    </row>
+    <row r="150" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="3">
+        <v>149</v>
+      </c>
+      <c r="B150" s="7">
+        <v>-25.413346199999999</v>
+      </c>
+      <c r="C150" s="7">
+        <v>-49.246321199999997</v>
+      </c>
+      <c r="D150" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="H150" s="7"/>
+      <c r="I150" s="7"/>
+      <c r="J150" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="K150" s="7"/>
+      <c r="L150" s="7"/>
+      <c r="M150" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N150" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O150" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P150" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q150" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="R150" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S150" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T150" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="3">
+        <v>150</v>
+      </c>
+      <c r="B151" s="7">
+        <v>-25.4400686</v>
+      </c>
+      <c r="C151" s="7">
+        <v>-49.2729967</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
+      <c r="G151" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="H151" s="7"/>
+      <c r="I151" s="7"/>
+      <c r="J151" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N151" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O151" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P151" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q151" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="R151" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S151" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T151" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="3">
+        <v>151</v>
+      </c>
+      <c r="B152" s="7">
+        <v>-25.4453639</v>
+      </c>
+      <c r="C152" s="7">
+        <v>-49.262008100000003</v>
+      </c>
+      <c r="D152" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7">
+        <v>847</v>
+      </c>
+      <c r="G152" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="H152" s="7"/>
+      <c r="I152" s="7"/>
+      <c r="J152" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K152" s="7"/>
+      <c r="L152" s="7"/>
+      <c r="M152" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N152" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O152" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P152" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q152" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="R152" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S152" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T152" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="3">
+        <v>152</v>
+      </c>
+      <c r="B153" s="7">
+        <v>-25.436912</v>
+      </c>
+      <c r="C153" s="7">
+        <v>-49.276989999999998</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7">
+        <v>41</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I153" s="7"/>
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N153" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O153" s="7"/>
+      <c r="P153" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q153" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="R153" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S153" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T153" s="7"/>
+    </row>
+    <row r="154" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="3">
+        <v>153</v>
+      </c>
+      <c r="B154" s="7">
+        <v>-25.448996600000001</v>
+      </c>
+      <c r="C154" s="7">
+        <v>-49.307680900000001</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="E154" s="7"/>
+      <c r="F154" s="7"/>
+      <c r="G154" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="H154" s="7"/>
+      <c r="I154" s="7"/>
+      <c r="J154" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="K154" s="7"/>
+      <c r="L154" s="7"/>
+      <c r="M154" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N154" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O154" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P154" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q154" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="R154" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S154" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T154" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="3">
+        <v>154</v>
+      </c>
+      <c r="B155" s="7">
+        <v>-25.459851799999999</v>
+      </c>
+      <c r="C155" s="7">
+        <v>-49.296717299999997</v>
+      </c>
+      <c r="D155" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7">
+        <v>709</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="H155" s="7"/>
+      <c r="I155" s="7"/>
+      <c r="J155" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N155" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O155" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P155" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q155" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="R155" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S155" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T155" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="3">
+        <v>155</v>
+      </c>
+      <c r="B156" s="7">
+        <v>-25.4344626</v>
+      </c>
+      <c r="C156" s="7">
+        <v>-49.279538799999997</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="E156" s="7"/>
+      <c r="F156" s="7">
+        <v>285</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H156" s="7"/>
+      <c r="I156" s="7"/>
+      <c r="J156" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K156" s="7"/>
+      <c r="L156" s="7"/>
+      <c r="M156" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N156" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O156" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P156" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q156" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="R156" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S156" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T156" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="3">
+        <v>156</v>
+      </c>
+      <c r="B157" s="7">
+        <v>-25.421608500000001</v>
+      </c>
+      <c r="C157" s="7">
+        <v>-49.269772400000001</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7"/>
+      <c r="G157" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H157" s="7"/>
+      <c r="I157" s="7"/>
+      <c r="J157" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K157" s="7"/>
+      <c r="L157" s="7"/>
+      <c r="M157" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N157" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O157" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P157" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q157" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="R157" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S157" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T157" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="3">
+        <v>157</v>
+      </c>
+      <c r="B158" s="7">
+        <v>-25.466983800000001</v>
+      </c>
+      <c r="C158" s="7">
+        <v>-49.280487600000001</v>
+      </c>
+      <c r="D158" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="E158" s="7"/>
+      <c r="F158" s="7">
+        <v>2532</v>
+      </c>
+      <c r="G158" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H158" s="7"/>
+      <c r="I158" s="7"/>
+      <c r="J158" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K158" s="7"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N158" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O158" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P158" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q158" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="R158" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S158" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T158" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="3">
+        <v>158</v>
+      </c>
+      <c r="B159" s="7">
+        <v>-25.430538800000001</v>
+      </c>
+      <c r="C159" s="7">
+        <v>-49.295968000000002</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
+      <c r="G159" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="H159" s="7"/>
+      <c r="I159" s="7"/>
+      <c r="J159" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K159" s="7"/>
+      <c r="L159" s="7"/>
+      <c r="M159" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N159" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O159" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P159" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q159" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="R159" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S159" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T159" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="3">
+        <v>159</v>
+      </c>
+      <c r="B160" s="7">
+        <v>-25.435370299999999</v>
+      </c>
+      <c r="C160" s="7">
+        <v>-49.313980100000002</v>
+      </c>
+      <c r="D160" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
+      <c r="G160" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="H160" s="7"/>
+      <c r="I160" s="7"/>
+      <c r="J160" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="K160" s="7"/>
+      <c r="L160" s="7"/>
+      <c r="M160" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N160" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O160" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P160" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q160" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="R160" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S160" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T160" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="3">
+        <v>160</v>
+      </c>
+      <c r="B161" s="7">
+        <v>-25.4917643</v>
+      </c>
+      <c r="C161" s="7">
+        <v>-49.2888254</v>
+      </c>
+      <c r="D161" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
+      <c r="G161" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="H161" s="7"/>
+      <c r="I161" s="7"/>
+      <c r="J161" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K161" s="7"/>
+      <c r="L161" s="7"/>
+      <c r="M161" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N161" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O161" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P161" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q161" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="R161" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S161" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T161" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="3">
+        <v>161</v>
+      </c>
+      <c r="B162" s="7">
+        <v>-25.477908100000001</v>
+      </c>
+      <c r="C162" s="7">
+        <v>-49.266559999999998</v>
+      </c>
+      <c r="D162" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E162" s="7"/>
+      <c r="F162" s="7">
+        <v>866</v>
+      </c>
+      <c r="G162" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H162" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I162" s="7"/>
+      <c r="J162" s="7"/>
+      <c r="K162" s="7"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N162" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O162" s="7"/>
+      <c r="P162" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q162" s="7"/>
+      <c r="R162" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S162" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T162" s="7"/>
+    </row>
+    <row r="163" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="3">
+        <v>162</v>
+      </c>
+      <c r="B163" s="7">
+        <v>-25.487290600000001</v>
+      </c>
+      <c r="C163" s="7">
+        <v>-49.301054600000001</v>
+      </c>
+      <c r="D163" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="H163" s="7"/>
+      <c r="I163" s="7"/>
+      <c r="J163" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K163" s="7"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N163" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O163" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P163" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q163" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="R163" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S163" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T163" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="3">
+        <v>163</v>
+      </c>
+      <c r="B164" s="7">
+        <v>-25.477601700000001</v>
+      </c>
+      <c r="C164" s="7">
+        <v>-49.292102900000003</v>
+      </c>
+      <c r="D164" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E164" s="7"/>
+      <c r="F164" s="7"/>
+      <c r="G164" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="H164" s="7"/>
+      <c r="I164" s="7"/>
+      <c r="J164" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K164" s="7"/>
+      <c r="L164" s="7"/>
+      <c r="M164" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N164" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O164" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P164" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q164" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="R164" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S164" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T164" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="3">
+        <v>164</v>
+      </c>
+      <c r="B165" s="7">
+        <v>-25.506892499999999</v>
+      </c>
+      <c r="C165" s="7">
+        <v>-49.304559500000003</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="E165" s="7"/>
+      <c r="F165" s="7"/>
+      <c r="G165" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="H165" s="7"/>
+      <c r="I165" s="7"/>
+      <c r="J165" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="K165" s="7"/>
+      <c r="L165" s="7"/>
+      <c r="M165" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N165" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O165" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P165" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q165" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="R165" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S165" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T165" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="3">
+        <v>165</v>
+      </c>
+      <c r="B166" s="7">
+        <v>-25.461393399999999</v>
+      </c>
+      <c r="C166" s="7">
+        <v>-49.325192600000001</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="E166" s="7"/>
+      <c r="F166" s="7"/>
+      <c r="G166" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="H166" s="7"/>
+      <c r="I166" s="7"/>
+      <c r="J166" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="K166" s="7"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N166" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O166" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P166" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q166" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="R166" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S166" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T166" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="3">
+        <v>166</v>
+      </c>
+      <c r="B167" s="7">
+        <v>-25.462443</v>
+      </c>
+      <c r="C167" s="7">
+        <v>-49.344991</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="E167" s="7"/>
+      <c r="F167" s="7">
+        <v>1569</v>
+      </c>
+      <c r="G167" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="H167" s="7"/>
+      <c r="I167" s="7"/>
+      <c r="J167" s="7"/>
+      <c r="K167" s="7"/>
+      <c r="L167" s="7"/>
+      <c r="M167" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N167" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O167" s="7"/>
+      <c r="P167" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q167" s="7"/>
+      <c r="R167" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S167" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T167" s="7"/>
+    </row>
+    <row r="168" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="3">
+        <v>167</v>
+      </c>
+      <c r="B168" s="7">
+        <v>-25.484921</v>
+      </c>
+      <c r="C168" s="7">
+        <v>-49.351852999999998</v>
+      </c>
+      <c r="D168" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="E168" s="7"/>
+      <c r="F168" s="7">
+        <v>2461</v>
+      </c>
+      <c r="G168" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="H168" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I168" s="7"/>
+      <c r="J168" s="7"/>
+      <c r="K168" s="7"/>
+      <c r="L168" s="7"/>
+      <c r="M168" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N168" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O168" s="7"/>
+      <c r="P168" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q168" s="7"/>
+      <c r="R168" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S168" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T168" s="7"/>
+    </row>
+    <row r="169" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="3">
+        <v>168</v>
+      </c>
+      <c r="B169" s="7">
+        <v>-25.445523999999999</v>
+      </c>
+      <c r="C169" s="7">
+        <v>-49.345993100000001</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="E169" s="7"/>
+      <c r="F169" s="7">
+        <v>4211</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="H169" s="7"/>
+      <c r="I169" s="7"/>
+      <c r="J169" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="K169" s="7"/>
+      <c r="L169" s="7"/>
+      <c r="M169" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N169" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O169" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P169" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q169" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="R169" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S169" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T169" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="3">
+        <v>169</v>
+      </c>
+      <c r="B170" s="7">
+        <v>-23.549302999999998</v>
+      </c>
+      <c r="C170" s="7">
+        <v>-46.483313000000003</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="E170" s="7"/>
+      <c r="F170" s="7">
+        <v>87</v>
+      </c>
+      <c r="G170" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="H170" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="I170" s="7"/>
+      <c r="J170" s="7"/>
+      <c r="K170" s="7"/>
+      <c r="L170" s="7"/>
+      <c r="M170" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="N170" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="O170" s="7"/>
+      <c r="P170" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q170" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="R170" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S170" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T170" s="7"/>
+    </row>
+    <row r="171" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="3">
+        <v>170</v>
+      </c>
+      <c r="B171" s="7">
+        <v>-21.781527000000001</v>
+      </c>
+      <c r="C171" s="7">
+        <v>-46.540058000000002</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="E171" s="7"/>
+      <c r="F171" s="7"/>
+      <c r="G171" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="H171" s="7"/>
+      <c r="I171" s="7"/>
+      <c r="J171" s="7"/>
+      <c r="K171" s="7"/>
+      <c r="L171" s="7"/>
+      <c r="M171" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="N171" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="O171" s="7"/>
+      <c r="P171" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q171" s="7"/>
+      <c r="R171" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S171" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T171" s="7"/>
+    </row>
+    <row r="172" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="3">
+        <v>171</v>
+      </c>
+      <c r="B172" s="7">
+        <v>-25.489768999999999</v>
+      </c>
+      <c r="C172" s="7">
+        <v>-49.332877500000002</v>
+      </c>
+      <c r="D172" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="E172" s="7"/>
+      <c r="F172" s="7"/>
+      <c r="G172" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="H172" s="7"/>
+      <c r="I172" s="7"/>
+      <c r="J172" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="K172" s="7"/>
+      <c r="L172" s="7"/>
+      <c r="M172" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N172" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O172" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P172" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q172" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="R172" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S172" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T172" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="3">
+        <v>172</v>
+      </c>
+      <c r="B173" s="7">
+        <v>-25.480015900000001</v>
+      </c>
+      <c r="C173" s="7">
+        <v>-49.3243717</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E173" s="7"/>
+      <c r="F173" s="7">
+        <v>2781</v>
+      </c>
+      <c r="G173" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="H173" s="7"/>
+      <c r="I173" s="7"/>
+      <c r="J173" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="K173" s="7"/>
+      <c r="L173" s="7"/>
+      <c r="M173" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N173" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O173" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P173" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q173" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="R173" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S173" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T173" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="3">
+        <v>173</v>
+      </c>
+      <c r="B174" s="7">
+        <v>-25.499368</v>
+      </c>
+      <c r="C174" s="7">
+        <v>-49.343567</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="E174" s="7"/>
+      <c r="F174" s="7">
+        <v>90</v>
+      </c>
+      <c r="G174" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="H174" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I174" s="7"/>
+      <c r="J174" s="7"/>
+      <c r="K174" s="7"/>
+      <c r="L174" s="7"/>
+      <c r="M174" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N174" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O174" s="7"/>
+      <c r="P174" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q174" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="R174" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S174" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T174" s="7"/>
+    </row>
+    <row r="175" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="3">
+        <v>174</v>
+      </c>
+      <c r="B175" s="7">
+        <v>-25.5624045</v>
+      </c>
+      <c r="C175" s="7">
+        <v>-49.339153099999997</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E175" s="7"/>
+      <c r="F175" s="7">
+        <v>337</v>
+      </c>
+      <c r="G175" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="H175" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="I175" s="7"/>
+      <c r="J175" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K175" s="7"/>
+      <c r="L175" s="7"/>
+      <c r="M175" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N175" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O175" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P175" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q175" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="R175" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S175" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T175" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="176" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="3">
+        <v>175</v>
+      </c>
+      <c r="B176" s="7">
+        <v>-25.5735888</v>
+      </c>
+      <c r="C176" s="7">
+        <v>-49.331338000000002</v>
+      </c>
+      <c r="D176" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7">
+        <v>1047</v>
+      </c>
+      <c r="G176" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="H176" s="7"/>
+      <c r="I176" s="7"/>
+      <c r="J176" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K176" s="7"/>
+      <c r="L176" s="7"/>
+      <c r="M176" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N176" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O176" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P176" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q176" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="R176" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S176" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T176" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="3">
+        <v>176</v>
+      </c>
+      <c r="B177" s="7">
+        <v>-25.586061600000001</v>
+      </c>
+      <c r="C177" s="7">
+        <v>-49.333774099999999</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="H177" s="7"/>
+      <c r="I177" s="7"/>
+      <c r="J177" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="K177" s="7"/>
+      <c r="L177" s="7"/>
+      <c r="M177" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N177" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O177" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P177" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q177" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="R177" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S177" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T177" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="3">
+        <v>177</v>
+      </c>
+      <c r="B178" s="7">
+        <v>-25.467976400000001</v>
+      </c>
+      <c r="C178" s="7">
+        <v>-49.241374999999998</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="E178" s="7"/>
+      <c r="F178" s="7">
+        <v>50</v>
+      </c>
+      <c r="G178" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="H178" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I178" s="7"/>
+      <c r="J178" s="7"/>
+      <c r="K178" s="7"/>
+      <c r="L178" s="7"/>
+      <c r="M178" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N178" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O178" s="7"/>
+      <c r="P178" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q178" s="7"/>
+      <c r="R178" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S178" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T178" s="7"/>
+    </row>
+    <row r="179" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="3">
+        <v>178</v>
+      </c>
+      <c r="B179" s="7">
+        <v>-19.741945000000001</v>
+      </c>
+      <c r="C179" s="7">
+        <v>-47.890127</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="E179" s="7"/>
+      <c r="F179" s="7">
+        <v>173</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="H179" s="7"/>
+      <c r="I179" s="7"/>
+      <c r="J179" s="7"/>
+      <c r="K179" s="7"/>
+      <c r="L179" s="7"/>
+      <c r="M179" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N179" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="O179" s="7"/>
+      <c r="P179" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q179" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="R179" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S179" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T179" s="7"/>
+    </row>
+    <row r="180" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="3">
+        <v>179</v>
+      </c>
+      <c r="B180" s="7">
+        <v>-25.4771961</v>
+      </c>
+      <c r="C180" s="7">
+        <v>-49.249163799999998</v>
+      </c>
+      <c r="D180" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="E180" s="7"/>
+      <c r="F180" s="7">
+        <v>5595</v>
+      </c>
+      <c r="G180" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H180" s="7"/>
+      <c r="I180" s="7"/>
+      <c r="J180" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="K180" s="7"/>
+      <c r="L180" s="7"/>
+      <c r="M180" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N180" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O180" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P180" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q180" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="R180" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S180" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T180" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="3">
+        <v>180</v>
+      </c>
+      <c r="B181" s="7">
+        <v>-25.500387400000001</v>
+      </c>
+      <c r="C181" s="7">
+        <v>-49.2351405</v>
+      </c>
+      <c r="D181" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="E181" s="7"/>
+      <c r="F181" s="7">
+        <v>707</v>
+      </c>
+      <c r="G181" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="H181" s="7"/>
+      <c r="I181" s="7"/>
+      <c r="J181" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K181" s="7"/>
+      <c r="L181" s="7"/>
+      <c r="M181" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N181" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O181" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P181" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q181" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="R181" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S181" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T181" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="3">
+        <v>181</v>
+      </c>
+      <c r="B182" s="7">
+        <v>-25.494415</v>
+      </c>
+      <c r="C182" s="7">
+        <v>-49.253501200000002</v>
+      </c>
+      <c r="D182" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
+      <c r="G182" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="H182" s="7"/>
+      <c r="I182" s="7"/>
+      <c r="J182" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K182" s="7"/>
+      <c r="L182" s="7"/>
+      <c r="M182" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N182" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O182" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P182" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q182" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="R182" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S182" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T182" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="3">
+        <v>182</v>
+      </c>
+      <c r="B183" s="7">
+        <v>-26.958438999999998</v>
+      </c>
+      <c r="C183" s="7">
+        <v>-52.524014000000001</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7">
+        <v>119</v>
+      </c>
+      <c r="G183" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="H183" s="7"/>
+      <c r="I183" s="7"/>
+      <c r="J183" s="7"/>
+      <c r="K183" s="7"/>
+      <c r="L183" s="7"/>
+      <c r="M183" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="N183" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="O183" s="7"/>
+      <c r="P183" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q183" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="R183" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S183" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T183" s="7"/>
+    </row>
+    <row r="184" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="3">
+        <v>183</v>
+      </c>
+      <c r="B184" s="7">
+        <v>-25.514084400000002</v>
+      </c>
+      <c r="C184" s="7">
+        <v>-49.2778195</v>
+      </c>
+      <c r="D184" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="E184" s="7"/>
+      <c r="F184" s="7">
+        <v>975</v>
+      </c>
+      <c r="G184" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="H184" s="7"/>
+      <c r="I184" s="7"/>
+      <c r="J184" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K184" s="7"/>
+      <c r="L184" s="7"/>
+      <c r="M184" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N184" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O184" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P184" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q184" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="R184" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S184" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T184" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="185" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A185" s="3">
+        <v>184</v>
+      </c>
+      <c r="B185" s="7">
+        <v>-25.528199000000001</v>
+      </c>
+      <c r="C185" s="7">
+        <v>-49.271457400000003</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="E185" s="7"/>
+      <c r="F185" s="7">
+        <v>79</v>
+      </c>
+      <c r="G185" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="H185" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I185" s="7"/>
+      <c r="J185" s="7"/>
+      <c r="K185" s="7"/>
+      <c r="L185" s="7"/>
+      <c r="M185" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N185" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O185" s="7"/>
+      <c r="P185" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q185" s="7"/>
+      <c r="R185" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S185" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T185" s="7"/>
+    </row>
+    <row r="186" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A186" s="3">
+        <v>185</v>
+      </c>
+      <c r="B186" s="7">
+        <v>-25.538886699999999</v>
+      </c>
+      <c r="C186" s="7">
+        <v>-49.253343100000002</v>
+      </c>
+      <c r="D186" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="E186" s="7"/>
+      <c r="F186" s="7"/>
+      <c r="G186" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H186" s="7"/>
+      <c r="I186" s="7"/>
+      <c r="J186" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K186" s="7"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N186" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O186" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P186" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q186" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="R186" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S186" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T186" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="3">
+        <v>186</v>
+      </c>
+      <c r="B187" s="7">
+        <v>-25.534249800000001</v>
+      </c>
+      <c r="C187" s="7">
+        <v>-49.257513799999998</v>
+      </c>
+      <c r="D187" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7">
+        <v>2433</v>
+      </c>
+      <c r="G187" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H187" s="7"/>
+      <c r="I187" s="7"/>
+      <c r="J187" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N187" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O187" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P187" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q187" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="R187" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S187" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T187" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="3">
+        <v>187</v>
+      </c>
+      <c r="B188" s="7">
+        <v>-25.5460101</v>
+      </c>
+      <c r="C188" s="7">
+        <v>-49.257148700000002</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="G188" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="H188" s="7"/>
+      <c r="I188" s="7"/>
+      <c r="J188" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K188" s="7"/>
+      <c r="L188" s="7"/>
+      <c r="M188" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N188" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O188" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P188" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q188" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="R188" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S188" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T188" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="189" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="3">
+        <v>188</v>
+      </c>
+      <c r="B189" s="7">
+        <v>-25.5504982</v>
+      </c>
+      <c r="C189" s="7">
+        <v>-49.268419100000003</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="E189" s="7"/>
+      <c r="F189" s="7"/>
+      <c r="G189" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H189" s="7"/>
+      <c r="I189" s="7"/>
+      <c r="J189" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K189" s="7"/>
+      <c r="L189" s="7"/>
+      <c r="M189" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N189" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O189" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P189" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q189" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="R189" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S189" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T189" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="190" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="3">
+        <v>189</v>
+      </c>
+      <c r="B190" s="7">
+        <v>-25.552745000000002</v>
+      </c>
+      <c r="C190" s="7">
+        <v>-49.2508342</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="E190" s="7"/>
+      <c r="F190" s="7"/>
+      <c r="G190" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="H190" s="7"/>
+      <c r="I190" s="7"/>
+      <c r="J190" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K190" s="7"/>
+      <c r="L190" s="7"/>
+      <c r="M190" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N190" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O190" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P190" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q190" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="R190" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S190" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T190" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="3">
+        <v>190</v>
+      </c>
+      <c r="B191" s="7">
+        <v>-25.567555899999999</v>
+      </c>
+      <c r="C191" s="7">
+        <v>-49.285356093441699</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="E191" s="7"/>
+      <c r="F191" s="7">
+        <v>4751</v>
+      </c>
+      <c r="G191" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="H191" s="7"/>
+      <c r="I191" s="7"/>
+      <c r="J191" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="K191" s="7"/>
+      <c r="L191" s="7"/>
+      <c r="M191" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N191" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O191" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P191" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q191" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="R191" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S191" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T191" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="3">
+        <v>191</v>
+      </c>
+      <c r="B192" s="7">
+        <v>-25.4223912</v>
+      </c>
+      <c r="C192" s="7">
+        <v>-49.319602400000001</v>
+      </c>
+      <c r="D192" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="E192" s="7"/>
+      <c r="F192" s="7"/>
+      <c r="G192" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="H192" s="7"/>
+      <c r="I192" s="7"/>
+      <c r="J192" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K192" s="7"/>
+      <c r="L192" s="7"/>
+      <c r="M192" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N192" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O192" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P192" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q192" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="R192" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S192" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T192" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="3">
+        <v>192</v>
+      </c>
+      <c r="B193" s="7">
+        <v>-25.401185999999999</v>
+      </c>
+      <c r="C193" s="7">
+        <v>-49.329189</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="E193" s="7"/>
+      <c r="F193" s="7"/>
+      <c r="G193" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="H193" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I193" s="7"/>
+      <c r="J193" s="7"/>
+      <c r="K193" s="7"/>
+      <c r="L193" s="7"/>
+      <c r="M193" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N193" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O193" s="7"/>
+      <c r="P193" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q193" s="7"/>
+      <c r="R193" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S193" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T193" s="7"/>
+    </row>
+    <row r="194" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="3">
+        <v>193</v>
+      </c>
+      <c r="B194" s="7">
+        <v>-25.387188200000001</v>
+      </c>
+      <c r="C194" s="7">
+        <v>-49.301633199999998</v>
+      </c>
+      <c r="D194" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E194" s="7"/>
+      <c r="F194" s="7"/>
+      <c r="G194" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="H194" s="7"/>
+      <c r="I194" s="7"/>
+      <c r="J194" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="K194" s="7"/>
+      <c r="L194" s="7"/>
+      <c r="M194" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N194" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O194" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P194" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q194" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="R194" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S194" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T194" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A195" s="3">
+        <v>194</v>
+      </c>
+      <c r="B195" s="7">
+        <v>-25.3876138</v>
+      </c>
+      <c r="C195" s="7">
+        <v>-49.267659199999997</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="E195" s="7"/>
+      <c r="F195" s="7"/>
+      <c r="G195" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H195" s="7"/>
+      <c r="I195" s="7"/>
+      <c r="J195" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="K195" s="7"/>
+      <c r="L195" s="7"/>
+      <c r="M195" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N195" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O195" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P195" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q195" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="R195" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S195" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T195" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="196" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A196" s="3">
+        <v>195</v>
+      </c>
+      <c r="B196" s="7">
+        <v>-25.3976489</v>
+      </c>
+      <c r="C196" s="7">
+        <v>-49.264652499999997</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="E196" s="7"/>
+      <c r="F196" s="7"/>
+      <c r="G196" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="H196" s="7"/>
+      <c r="I196" s="7"/>
+      <c r="J196" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="K196" s="7"/>
+      <c r="L196" s="7"/>
+      <c r="M196" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N196" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O196" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P196" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q196" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="R196" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S196" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T196" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="197" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="3">
+        <v>196</v>
+      </c>
+      <c r="B197" s="7">
+        <v>-25.371727</v>
+      </c>
+      <c r="C197" s="7">
+        <v>-49.262377999999998</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="E197" s="7"/>
+      <c r="F197" s="7">
+        <v>2</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="H197" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I197" s="7"/>
+      <c r="J197" s="7"/>
+      <c r="K197" s="7"/>
+      <c r="L197" s="7"/>
+      <c r="M197" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N197" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O197" s="7"/>
+      <c r="P197" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q197" s="7"/>
+      <c r="R197" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S197" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T197" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="198" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="3">
+        <v>197</v>
+      </c>
+      <c r="B198" s="7">
+        <v>-25.418295799999999</v>
+      </c>
+      <c r="C198" s="7">
+        <v>-49.348520299999997</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="E198" s="7"/>
+      <c r="F198" s="7">
+        <v>3225</v>
+      </c>
+      <c r="G198" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H198" s="7"/>
+      <c r="I198" s="7"/>
+      <c r="J198" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="M198" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N198" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O198" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P198" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q198" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="R198" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S198" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T198" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="199" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A199" s="3">
+        <v>198</v>
+      </c>
+      <c r="B199" s="7">
+        <v>-19.309512000000002</v>
+      </c>
+      <c r="C199" s="7">
+        <v>-40.684733999999999</v>
+      </c>
+      <c r="D199" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="E199" s="7"/>
+      <c r="F199" s="7"/>
+      <c r="G199" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="H199" s="7"/>
+      <c r="I199" s="7"/>
+      <c r="J199" s="7"/>
+      <c r="K199" s="7"/>
+      <c r="L199" s="7"/>
+      <c r="M199" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="N199" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="O199" s="7"/>
+      <c r="P199" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q199" s="7"/>
+      <c r="R199" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S199" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T199" s="7"/>
+    </row>
+    <row r="200" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A200" s="3">
+        <v>199</v>
+      </c>
+      <c r="B200" s="7">
+        <v>-25.384296500000001</v>
+      </c>
+      <c r="C200" s="7">
+        <v>-49.334810500000003</v>
+      </c>
+      <c r="D200" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="E200" s="7"/>
+      <c r="F200" s="7"/>
+      <c r="G200" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H200" s="7"/>
+      <c r="I200" s="7"/>
+      <c r="J200" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K200" s="7"/>
+      <c r="L200" s="7"/>
+      <c r="M200" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N200" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O200" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P200" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q200" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="R200" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S200" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T200" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="201" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A201" s="3">
+        <v>200</v>
+      </c>
+      <c r="B201" s="7">
+        <v>-25.4111735</v>
+      </c>
+      <c r="C201" s="7">
+        <v>-49.237539900000002</v>
+      </c>
+      <c r="D201" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E201" s="7"/>
+      <c r="F201" s="7"/>
+      <c r="G201" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="H201" s="7"/>
+      <c r="I201" s="7"/>
+      <c r="J201" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K201" s="7"/>
+      <c r="L201" s="7"/>
+      <c r="M201" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N201" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O201" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P201" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q201" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="R201" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S201" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T201" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="3">
+        <v>201</v>
+      </c>
+      <c r="B202" s="7">
+        <v>-25.383946099999999</v>
+      </c>
+      <c r="C202" s="7">
+        <v>-49.247129399999999</v>
+      </c>
+      <c r="D202" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="E202" s="7"/>
+      <c r="F202" s="7"/>
+      <c r="G202" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="H202" s="7"/>
+      <c r="I202" s="7"/>
+      <c r="J202" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="K202" s="7"/>
+      <c r="L202" s="7"/>
+      <c r="M202" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N202" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O202" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P202" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q202" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="R202" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S202" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T202" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="3">
+        <v>202</v>
+      </c>
+      <c r="B203" s="7">
+        <v>-25.373726000000001</v>
+      </c>
+      <c r="C203" s="7">
+        <v>-49.218851000000001</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="E203" s="7"/>
+      <c r="F203" s="7">
+        <v>90</v>
+      </c>
+      <c r="G203" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="H203" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="I203" s="7"/>
+      <c r="J203" s="7"/>
+      <c r="K203" s="7"/>
+      <c r="L203" s="7"/>
+      <c r="M203" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N203" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O203" s="7"/>
+      <c r="P203" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q203" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="R203" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S203" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T203" s="7"/>
+    </row>
+    <row r="204" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A204" s="3">
+        <v>203</v>
+      </c>
+      <c r="B204" s="7">
+        <v>-25.368722999999999</v>
+      </c>
+      <c r="C204" s="7">
+        <v>-49.236659699999997</v>
+      </c>
+      <c r="D204" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="E204" s="7"/>
+      <c r="F204" s="7">
+        <v>1542</v>
+      </c>
+      <c r="G204" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="H204" s="7"/>
+      <c r="I204" s="7"/>
+      <c r="J204" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="K204" s="7"/>
+      <c r="L204" s="7"/>
+      <c r="M204" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N204" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O204" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P204" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q204" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="R204" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S204" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T204" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A205" s="3">
+        <v>204</v>
+      </c>
+      <c r="B205" s="7">
+        <v>24.816579999999998</v>
+      </c>
+      <c r="C205" s="7">
+        <v>-107.56234000000001</v>
+      </c>
+      <c r="D205" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
+      <c r="G205" s="7"/>
+      <c r="H205" s="7"/>
+      <c r="I205" s="7"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="N205" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="O205" s="7"/>
+      <c r="P205" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q205" s="7"/>
+      <c r="R205" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="S205" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="T205" s="7"/>
+    </row>
+    <row r="206" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="3">
+        <v>205</v>
+      </c>
+      <c r="B206" s="7">
+        <v>-25.443344100000001</v>
+      </c>
+      <c r="C206" s="7">
+        <v>-49.208508500000001</v>
+      </c>
+      <c r="D206" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E206" s="7"/>
+      <c r="F206" s="7"/>
+      <c r="G206" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H206" s="7"/>
+      <c r="I206" s="7"/>
+      <c r="J206" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K206" s="7"/>
+      <c r="L206" s="7"/>
+      <c r="M206" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N206" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O206" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P206" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q206" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="R206" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S206" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T206" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="3">
+        <v>206</v>
+      </c>
+      <c r="B207" s="7">
+        <v>-25.4209496</v>
+      </c>
+      <c r="C207" s="7">
+        <v>-49.207515999999998</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="E207" s="7"/>
+      <c r="F207" s="7"/>
+      <c r="G207" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="H207" s="7"/>
+      <c r="I207" s="7"/>
+      <c r="J207" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="K207" s="7"/>
+      <c r="L207" s="7"/>
+      <c r="M207" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N207" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O207" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P207" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q207" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="R207" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S207" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T207" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="3">
+        <v>207</v>
+      </c>
+      <c r="B208" s="7">
+        <v>-25.4135642</v>
+      </c>
+      <c r="C208" s="7">
+        <v>-49.209688300000003</v>
+      </c>
+      <c r="D208" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="E208" s="7"/>
+      <c r="F208" s="7"/>
+      <c r="G208" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="H208" s="7"/>
+      <c r="I208" s="7"/>
+      <c r="J208" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="K208" s="7"/>
+      <c r="L208" s="7"/>
+      <c r="M208" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N208" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O208" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P208" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q208" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="R208" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S208" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T208" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="3">
+        <v>208</v>
+      </c>
+      <c r="B209" s="7">
+        <v>-25.459967800000001</v>
+      </c>
+      <c r="C209" s="7">
+        <v>-49.196872800000001</v>
+      </c>
+      <c r="D209" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="E209" s="7"/>
+      <c r="F209" s="7"/>
+      <c r="G209" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="H209" s="7"/>
+      <c r="I209" s="7"/>
+      <c r="J209" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K209" s="7"/>
+      <c r="L209" s="7"/>
+      <c r="M209" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N209" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O209" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P209" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q209" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="R209" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S209" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T209" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A210" s="3">
+        <v>209</v>
+      </c>
+      <c r="B210" s="7">
+        <v>-25.451671900000001</v>
+      </c>
+      <c r="C210" s="7">
+        <v>-49.219061500000002</v>
+      </c>
+      <c r="D210" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E210" s="7"/>
+      <c r="F210" s="7">
+        <v>1616</v>
+      </c>
+      <c r="G210" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="H210" s="7"/>
+      <c r="I210" s="7"/>
+      <c r="J210" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K210" s="7"/>
+      <c r="L210" s="7"/>
+      <c r="M210" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N210" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O210" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P210" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q210" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="R210" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S210" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T210" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A211" s="3">
+        <v>210</v>
+      </c>
+      <c r="B211" s="7">
+        <v>-25.469188800000001</v>
+      </c>
+      <c r="C211" s="7">
+        <v>-49.204248100000001</v>
+      </c>
+      <c r="D211" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="E211" s="7"/>
+      <c r="F211" s="7"/>
+      <c r="G211" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="H211" s="7"/>
+      <c r="I211" s="7"/>
+      <c r="J211" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K211" s="7"/>
+      <c r="L211" s="7"/>
+      <c r="M211" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N211" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O211" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P211" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q211" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="R211" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S211" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T211" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>